<commit_message>
generating animations for presentation
</commit_message>
<xml_diff>
--- a/Experiment/Experiment.xlsx
+++ b/Experiment/Experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478E7C0D-93C4-4B84-BA85-5B102E784EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE70BA6-8787-4BCB-9D2B-B308BFA078F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="837" firstSheet="2" activeTab="8" xr2:uid="{9618EC4A-BAF2-4511-9F63-3241D4476D9E}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="837" firstSheet="5" activeTab="14" xr2:uid="{9618EC4A-BAF2-4511-9F63-3241D4476D9E}"/>
   </bookViews>
   <sheets>
     <sheet name="movement1 40rpm" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,6 @@
     <sheet name="movement8 6rpm 15x20 (2)" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41580,7 +41579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2FC552-5866-4A71-8190-BCDF3D8C8D36}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -47217,7 +47216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CC8BDB-0236-41C6-9547-DB53C35B0BAF}">
   <dimension ref="B1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>